<commit_message>
refactored states by group
</commit_message>
<xml_diff>
--- a/Transition Table.xlsx
+++ b/Transition Table.xlsx
@@ -43,19 +43,19 @@
     <t xml:space="preserve">Password</t>
   </si>
   <si>
+    <t xml:space="preserve">Timer Runs Out</t>
+  </si>
+  <si>
     <t xml:space="preserve">Timer Ticks</t>
   </si>
   <si>
-    <t xml:space="preserve">Timer Runs Out</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ready</t>
   </si>
   <si>
-    <t xml:space="preserve">Arming (away)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arming (stay)</t>
+    <t xml:space="preserve">Arming (Away)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arming (Stay)</t>
   </si>
   <si>
     <t xml:space="preserve">~</t>
@@ -64,28 +64,28 @@
     <t xml:space="preserve">Unarmed</t>
   </si>
   <si>
-    <t xml:space="preserve">Confirm (away)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Confirm (stay)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Armed (away)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Armed (stay)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Disarm (away)</t>
+    <t xml:space="preserve">Confirm (Away)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confirm (Stay)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Armed (Away)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Armed (Stay)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disarm (Away)</t>
   </si>
   <si>
     <t xml:space="preserve">Warning</t>
   </si>
   <si>
-    <t xml:space="preserve">Disarm (stay)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Breach</t>
+    <t xml:space="preserve">Disarm (Stay)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Breached</t>
   </si>
 </sst>
 </file>
@@ -211,14 +211,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="13.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="15.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -308,10 +308,10 @@
         <v>12</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -340,10 +340,10 @@
         <v>12</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -476,7 +476,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>12</v>
@@ -500,15 +500,15 @@
         <v>13</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>12</v>
@@ -532,7 +532,7 @@
         <v>13</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>12</v>
@@ -540,7 +540,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>12</v>
@@ -564,15 +564,15 @@
         <v>13</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>12</v>
@@ -599,7 +599,7 @@
         <v>12</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
every thing almost done
</commit_message>
<xml_diff>
--- a/Transition Table.xlsx
+++ b/Transition Table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="23595" windowHeight="13650" tabRatio="500"/>
+    <workbookView windowWidth="22395" windowHeight="11400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -82,12 +82,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -102,7 +102,59 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -113,68 +165,34 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -186,6 +204,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -203,59 +235,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -270,187 +265,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -461,6 +456,36 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -488,6 +513,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -505,39 +539,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -550,152 +556,141 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -713,7 +708,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1038,7 +1033,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6095238095238" defaultRowHeight="12.75"/>

</xml_diff>